<commit_message>
Interactables, Door and collision audio
</commit_message>
<xml_diff>
--- a/HorrorGame/Assets/Audio/AudioFiles.xlsx
+++ b/HorrorGame/Assets/Audio/AudioFiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\skola\CVUT\Bachelors Project\bachelorsProject\HorrorGame\Assets\Audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71438B1A-3FB0-4018-8FD0-3B9ABE03280B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA15005-6E66-4076-B4CF-FDC5E0572042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="111">
   <si>
     <t>Name</t>
   </si>
@@ -259,6 +259,105 @@
   </si>
   <si>
     <t>556952__sami-hiltunen__horror-sfx-02.wav</t>
+  </si>
+  <si>
+    <t>Gate opening</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/joedeshon/sounds/339184/</t>
+  </si>
+  <si>
+    <t>339184__joedeshon__squeak-01.wav</t>
+  </si>
+  <si>
+    <t>Trimmed</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/DWOBoyle/sounds/144286/</t>
+  </si>
+  <si>
+    <t>Electric box</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/DWOBoyle/sounds/144284/</t>
+  </si>
+  <si>
+    <t>144286__dwoboyle__light-switch-0002-on-02.wav</t>
+  </si>
+  <si>
+    <t>144284__dwoboyle__light-switch-0003-off.wav</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/kwahmah_02/sounds/256116/</t>
+  </si>
+  <si>
+    <t>Mouse click</t>
+  </si>
+  <si>
+    <t>256116__kwahmah-02__click.wav</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/InspectorJ/sounds/337450/</t>
+  </si>
+  <si>
+    <t>Door squeak</t>
+  </si>
+  <si>
+    <t>337450__inspectorj__door-squeak-loud-a.wav</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/EminYILDIRIM/sounds/536076/</t>
+  </si>
+  <si>
+    <t>536076__eminyildirim__door-squeak.wav</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/stereostereo/sounds/124535/</t>
+  </si>
+  <si>
+    <t>124535__stereostereo__st-squeak-door.aiff</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/FullMetalJedi/sounds/390964/</t>
+  </si>
+  <si>
+    <t>Lab door</t>
+  </si>
+  <si>
+    <t>390964__fullmetaljedi__alarm02.wav</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/birdOfTheNorth/sounds/613290/</t>
+  </si>
+  <si>
+    <t>Collision / thud</t>
+  </si>
+  <si>
+    <t>613290__birdofthenorth__bassy-thud.wav</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/nebulasnails/sounds/405535/</t>
+  </si>
+  <si>
+    <t>405535__nebulasnails__thud-4.wav</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/OtisJames/sounds/215162/</t>
+  </si>
+  <si>
+    <t>215162__otisjames__thud.wav</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/nebulasnails/sounds/405537/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/nebulasnails/sounds/405536/</t>
+  </si>
+  <si>
+    <t>405537__nebulasnails__thud-2.wav</t>
+  </si>
+  <si>
+    <t>405536__nebulasnails__thud-3.wav</t>
   </si>
 </sst>
 </file>
@@ -325,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -335,6 +434,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
@@ -616,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,60 +1225,336 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1257,8 +1633,47 @@
     <hyperlink ref="D25" r:id="rId73" xr:uid="{E287107A-CE53-4339-9601-2AEE217A283F}"/>
     <hyperlink ref="D26" r:id="rId74" xr:uid="{6436DFBC-2293-47B5-86F7-D1B619E0CE12}"/>
     <hyperlink ref="E26" r:id="rId75" xr:uid="{DC84A2A0-7EC4-42A9-A3B1-C7042BEF8C9A}"/>
+    <hyperlink ref="C27" r:id="rId76" xr:uid="{C94488F7-07DB-4916-BEA9-B6DB6FDE36DD}"/>
+    <hyperlink ref="D27" r:id="rId77" xr:uid="{F37EFDC9-1DF2-4000-B650-A3B9AE118769}"/>
+    <hyperlink ref="E27" r:id="rId78" xr:uid="{C74C3ECF-0C0C-4068-910C-EAE8554C8620}"/>
+    <hyperlink ref="D28" r:id="rId79" xr:uid="{8765E8E6-EDA0-4C2E-A1E8-0E07CD9C7935}"/>
+    <hyperlink ref="C28" r:id="rId80" xr:uid="{81BE556D-B914-4C78-AA20-3FFDFD97BD4E}"/>
+    <hyperlink ref="E28" r:id="rId81" xr:uid="{C9D91D1F-16B7-41A4-80B1-EA1E649AC4C9}"/>
+    <hyperlink ref="D29" r:id="rId82" xr:uid="{ECEB1367-E0E4-412B-9D28-32EFB1B09DD0}"/>
+    <hyperlink ref="C29" r:id="rId83" xr:uid="{B3857C5C-9B2D-4D2F-AEE8-04DC05D251F2}"/>
+    <hyperlink ref="E29" r:id="rId84" xr:uid="{951EDC12-6E0E-4433-B991-F0DF07B38B57}"/>
+    <hyperlink ref="C30" r:id="rId85" xr:uid="{BDDB982C-FAB2-449A-A483-6F6D131BDDA9}"/>
+    <hyperlink ref="E30" r:id="rId86" xr:uid="{09EAAD66-E3D7-441D-B04B-6C004AC15CCC}"/>
+    <hyperlink ref="D30" r:id="rId87" xr:uid="{04FFBB14-C94E-4160-88C5-B3055D60F3FB}"/>
+    <hyperlink ref="D31" r:id="rId88" xr:uid="{8910E949-ED00-441E-BC59-9CD6D10BF07F}"/>
+    <hyperlink ref="E31" r:id="rId89" xr:uid="{F11EC8A9-F1E4-4D94-9EDF-61966CD73F82}"/>
+    <hyperlink ref="C31" r:id="rId90" xr:uid="{3C2A37B6-2C5B-4B7A-BFA7-C1710C2F8103}"/>
+    <hyperlink ref="D32" r:id="rId91" xr:uid="{018328DA-78D8-43DF-A106-0A8D93E9D48F}"/>
+    <hyperlink ref="C32" r:id="rId92" xr:uid="{3AFC31C7-F940-4DD2-BC94-06DF9CB93B56}"/>
+    <hyperlink ref="E32" r:id="rId93" xr:uid="{EBB781CA-B554-43B2-8815-1253BDA6EA85}"/>
+    <hyperlink ref="D33" r:id="rId94" xr:uid="{19E794AE-569C-4152-92EF-525B510EA0A2}"/>
+    <hyperlink ref="C33" r:id="rId95" xr:uid="{31651AB9-7ACB-49DC-9A2E-E46BAFC49A19}"/>
+    <hyperlink ref="E33" r:id="rId96" xr:uid="{5EB1ACCD-F9CE-495A-84D1-7A96020AA929}"/>
+    <hyperlink ref="D34" r:id="rId97" xr:uid="{DE4A266B-EA65-4441-BC67-90301F73FE0A}"/>
+    <hyperlink ref="C34" r:id="rId98" xr:uid="{097F42E2-DB56-421C-BF2B-64676D013847}"/>
+    <hyperlink ref="E34" r:id="rId99" xr:uid="{899F4FA9-0E0C-446C-A5A4-6E0FF5E7AF87}"/>
+    <hyperlink ref="D35" r:id="rId100" xr:uid="{7E33C556-C47B-4EAB-A88A-7DD3F1326A84}"/>
+    <hyperlink ref="C35" r:id="rId101" xr:uid="{3AAB6DD8-B4EA-400A-AE72-603B7FE17A97}"/>
+    <hyperlink ref="C36" r:id="rId102" xr:uid="{D9D90F66-21BE-4C05-BF81-8769D91956FC}"/>
+    <hyperlink ref="D36" r:id="rId103" xr:uid="{DBDC2A88-3B09-453B-96C8-F90F11547517}"/>
+    <hyperlink ref="E36" r:id="rId104" xr:uid="{0ED2AC43-4B61-4F30-A4C2-D557CD2C2FB2}"/>
+    <hyperlink ref="E35" r:id="rId105" xr:uid="{D008DE06-1825-44B9-B279-ED6DEBFC2302}"/>
+    <hyperlink ref="D37" r:id="rId106" xr:uid="{159D8439-754A-4083-8163-2B0BB64FC61E}"/>
+    <hyperlink ref="C37" r:id="rId107" xr:uid="{40F6B21B-C883-4DC0-90BC-903719FF73D5}"/>
+    <hyperlink ref="E37" r:id="rId108" xr:uid="{89882F9C-A31C-4792-B8CD-57E27E2DA9C5}"/>
+    <hyperlink ref="D38" r:id="rId109" xr:uid="{DE947725-211C-4E57-B345-AEEF9E842913}"/>
+    <hyperlink ref="C38" r:id="rId110" xr:uid="{1DA375B6-2C1B-4B5B-80C3-B72F54168AB4}"/>
+    <hyperlink ref="D39" r:id="rId111" xr:uid="{968FA50A-AD92-459F-A14E-FA090F288EA1}"/>
+    <hyperlink ref="E38" r:id="rId112" xr:uid="{7ADDC187-F89E-4FE0-9AE8-3DAC280959E6}"/>
+    <hyperlink ref="E39" r:id="rId113" xr:uid="{3564A8FE-606D-4A57-AAC6-1CA45B3FA4EE}"/>
+    <hyperlink ref="C39" r:id="rId114" xr:uid="{0034CD97-470B-4F26-9BFB-B3A24354C52D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId76"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId115"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Audio enhancements, level fixes, bug fixes
</commit_message>
<xml_diff>
--- a/HorrorGame/Assets/Audio/AudioFiles.xlsx
+++ b/HorrorGame/Assets/Audio/AudioFiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\skola\CVUT\Bachelors Project\bachelorsProject\HorrorGame\Assets\Audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB3F393-F530-4BE6-8009-22104EECB764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B20BB88-DD7D-42EC-82D8-FA190EEF3D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="126">
   <si>
     <t>Name</t>
   </si>
@@ -385,6 +385,24 @@
   </si>
   <si>
     <t>133974__mrpokephile__horrific-zombie-growl.mp3</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Jacco18/sounds/419023/</t>
+  </si>
+  <si>
+    <t>No lab card</t>
+  </si>
+  <si>
+    <t>419023__jacco18__acess-denied-buzz.mp3</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/stk13/sounds/121980/</t>
+  </si>
+  <si>
+    <t>Ambient music</t>
+  </si>
+  <si>
+    <t>121980__stk13__jungle-ninja.wav</t>
   </si>
 </sst>
 </file>
@@ -746,7 +764,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,19 +1578,39 @@
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
+      <c r="A45" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1751,8 +1789,14 @@
     <hyperlink ref="D43" r:id="rId124" xr:uid="{2C47B39F-CC7C-44B7-B071-9DE285CE8D4B}"/>
     <hyperlink ref="C43" r:id="rId125" xr:uid="{6B6D8024-B88D-47D9-89BB-B5E601BF520D}"/>
     <hyperlink ref="E43" r:id="rId126" xr:uid="{33750801-8F5B-49F0-B6F8-27DB77AF6505}"/>
+    <hyperlink ref="D44" r:id="rId127" xr:uid="{3D588524-D705-4C34-8057-58E931E0DFF7}"/>
+    <hyperlink ref="C44" r:id="rId128" xr:uid="{28C4E742-D754-42AA-8434-496C36B921FC}"/>
+    <hyperlink ref="E44" r:id="rId129" xr:uid="{11FEECD5-1D5D-40E7-9342-FB566C8FAD83}"/>
+    <hyperlink ref="D45" r:id="rId130" xr:uid="{643CF298-FAB8-4D7B-A868-480DE588628B}"/>
+    <hyperlink ref="C45" r:id="rId131" xr:uid="{2400831D-3FEB-4299-AC86-B1F79044C0F2}"/>
+    <hyperlink ref="E45" r:id="rId132" xr:uid="{1780D338-C96B-42CB-A7C2-E33C200AB344}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId127"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId133"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Death screen, click sound, bug fixes, adjusted pickup object
</commit_message>
<xml_diff>
--- a/HorrorGame/Assets/Audio/AudioFiles.xlsx
+++ b/HorrorGame/Assets/Audio/AudioFiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\skola\CVUT\Bachelors Project\bachelorsProject\HorrorGame\Assets\Audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B20BB88-DD7D-42EC-82D8-FA190EEF3D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066708C6-88D8-4E12-AF50-F34C66312C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="129">
   <si>
     <t>Name</t>
   </si>
@@ -403,6 +403,15 @@
   </si>
   <si>
     <t>121980__stk13__jungle-ninja.wav</t>
+  </si>
+  <si>
+    <t>448081__breviceps__tic-toc-click.wav</t>
+  </si>
+  <si>
+    <t>Menu UI Click</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Breviceps/sounds/448081/</t>
   </si>
 </sst>
 </file>
@@ -763,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="B35" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,11 +1623,21 @@
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1795,8 +1814,11 @@
     <hyperlink ref="D45" r:id="rId130" xr:uid="{643CF298-FAB8-4D7B-A868-480DE588628B}"/>
     <hyperlink ref="C45" r:id="rId131" xr:uid="{2400831D-3FEB-4299-AC86-B1F79044C0F2}"/>
     <hyperlink ref="E45" r:id="rId132" xr:uid="{1780D338-C96B-42CB-A7C2-E33C200AB344}"/>
+    <hyperlink ref="C46" r:id="rId133" xr:uid="{0AD478D4-457D-43C6-8C86-6CD72283A3E0}"/>
+    <hyperlink ref="E46" r:id="rId134" xr:uid="{54DBC843-9C87-404B-A9E8-77C4337A1522}"/>
+    <hyperlink ref="D46" r:id="rId135" xr:uid="{43D41189-14E5-45F8-9FDE-B09D5240C6D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId133"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId136"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Settings, fixed cursor bug, fixed hitting through doors bug
</commit_message>
<xml_diff>
--- a/HorrorGame/Assets/Audio/AudioFiles.xlsx
+++ b/HorrorGame/Assets/Audio/AudioFiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\skola\CVUT\Bachelors Project\bachelorsProject\HorrorGame\Assets\Audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B0C76A-6B90-4581-8AC9-B5E6E1DE2122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F83FCA26-18C1-4FE5-9C40-78FE64FA4BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -763,7 +763,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,22 +806,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -851,264 +851,264 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>86</v>
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>97</v>
+        <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>117</v>
+        <v>43</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>118</v>
+        <v>52</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>76</v>
+      <c r="A14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>106</v>
+      <c r="C15" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>21</v>
@@ -1118,379 +1118,383 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>66</v>
+      <c r="C16" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>35</v>
+      <c r="C17" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>34</v>
+      <c r="C18" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>86</v>
+      <c r="C23" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>86</v>
+      <c r="C24" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>86</v>
+      <c r="C25" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>92</v>
+        <v>33</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G26" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G28" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G29" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>43</v>
+      <c r="A30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>86</v>
+      <c r="C32" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>21</v>
@@ -1500,63 +1504,67 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G33" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>21</v>
@@ -1566,67 +1574,65 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>15</v>
+        <v>118</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>14</v>
@@ -1636,19 +1642,19 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>21</v>
@@ -1658,74 +1664,68 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1851,133 +1851,133 @@
   </sheetData>
   <autoFilter ref="A1:G49" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G49">
-      <sortCondition ref="E1:E49"/>
+      <sortCondition ref="C1:C49"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D42" r:id="rId1" xr:uid="{AB31DAB3-9BD1-4F3A-9C67-266253A7FBC9}"/>
-    <hyperlink ref="F42" r:id="rId2" xr:uid="{FA265D1A-7467-4D20-B06B-A57A3A3B9EC0}"/>
-    <hyperlink ref="E42" r:id="rId3" xr:uid="{8D565E7A-162F-4936-A87E-9067AF1B32C5}"/>
-    <hyperlink ref="D19" r:id="rId4" xr:uid="{14A7163B-E0A4-4CF0-8580-81B5F9151720}"/>
-    <hyperlink ref="E19" r:id="rId5" xr:uid="{F387424D-DD4F-4D43-A515-31E7B2F7E60D}"/>
-    <hyperlink ref="F19" r:id="rId6" xr:uid="{3FCC6F7F-7E77-45C4-80F3-37006936007B}"/>
-    <hyperlink ref="F36" r:id="rId7" xr:uid="{961C82C8-9EE0-4CC7-969E-429E97604A44}"/>
-    <hyperlink ref="D36" r:id="rId8" xr:uid="{29E5C07C-485E-4705-86A5-0805773A71FA}"/>
-    <hyperlink ref="E36" r:id="rId9" xr:uid="{845774F5-18E8-48D6-B185-5EADFEDD176A}"/>
-    <hyperlink ref="E7" r:id="rId10" xr:uid="{86FF1527-77B3-40A2-AC7A-466808CD627A}"/>
-    <hyperlink ref="F7" r:id="rId11" xr:uid="{97C35A04-8C6F-4B13-94DA-27ABEF4EA1A8}"/>
-    <hyperlink ref="D7" r:id="rId12" xr:uid="{DD99B592-4376-4718-B535-8D363D6F4F91}"/>
-    <hyperlink ref="E41" r:id="rId13" xr:uid="{43A44B70-53DA-45DC-96A6-100EB60E6E25}"/>
-    <hyperlink ref="D41" r:id="rId14" xr:uid="{3D4DEEB4-BBA8-42D4-86DE-41C6ECAE8658}"/>
-    <hyperlink ref="F41" r:id="rId15" xr:uid="{E4A64751-9876-494E-894F-EEBFD4AAA2DC}"/>
-    <hyperlink ref="E40" r:id="rId16" xr:uid="{59F4CE5E-9EDB-422C-9561-4B989B3F1BB9}"/>
-    <hyperlink ref="D40" r:id="rId17" xr:uid="{79BB2680-5EFF-4125-9139-09B0EA7840A3}"/>
-    <hyperlink ref="F40" r:id="rId18" xr:uid="{3999E02F-5F6D-49A0-B5C2-E49C775D9A0F}"/>
-    <hyperlink ref="E22" r:id="rId19" xr:uid="{902A354B-3B37-401E-AC8F-7E8BEF8D1480}"/>
-    <hyperlink ref="D22" r:id="rId20" xr:uid="{59AE041E-9814-4B37-92D2-6FB6B6358F14}"/>
-    <hyperlink ref="F22" r:id="rId21" xr:uid="{E0EFE0A8-5B37-4341-AE96-D9068EDDDD1D}"/>
-    <hyperlink ref="E12" r:id="rId22" xr:uid="{DD490B8D-8DC3-4D71-9E8A-0ECBF447F2C6}"/>
-    <hyperlink ref="D12" r:id="rId23" xr:uid="{5D43292E-C65D-4235-B9FD-0CEFF1E811F7}"/>
-    <hyperlink ref="F12" r:id="rId24" xr:uid="{04D35B6E-9D8A-4916-9692-3C5F3E598C19}"/>
-    <hyperlink ref="E18" r:id="rId25" xr:uid="{9AA0D1C7-90F7-4A2E-AA56-2F5442EC7372}"/>
-    <hyperlink ref="D18" r:id="rId26" xr:uid="{5CA1E2FE-E496-49DE-AA8F-E09FB87CB01B}"/>
-    <hyperlink ref="F18" r:id="rId27" xr:uid="{80AAC719-1D00-4D06-BCE4-7051130B5E4C}"/>
-    <hyperlink ref="F17" r:id="rId28" xr:uid="{96B8B0E9-437A-4600-888F-086253A894AC}"/>
-    <hyperlink ref="D17" r:id="rId29" xr:uid="{C23ACE2A-9613-465E-9C5F-D0DB9CB85A71}"/>
-    <hyperlink ref="E17" r:id="rId30" xr:uid="{8E3C6832-26BE-4E46-BB46-BC801F2F73B4}"/>
-    <hyperlink ref="E37" r:id="rId31" xr:uid="{7F34C4E1-B864-4826-9C06-D9B5AC94F1E8}"/>
-    <hyperlink ref="D37" r:id="rId32" xr:uid="{38FF4FD6-EE0D-4CB9-A9A3-48FF37E7358D}"/>
-    <hyperlink ref="F37" r:id="rId33" xr:uid="{1533D866-2B4B-47F8-8F74-C3C814BBBD09}"/>
-    <hyperlink ref="D27" r:id="rId34" xr:uid="{AC2B16DC-1EC4-4B44-A10B-3930A7203AAD}"/>
-    <hyperlink ref="E27" r:id="rId35" xr:uid="{AB5148A2-9F1E-4BDC-8A6B-8FAE98A5E4B5}"/>
-    <hyperlink ref="F27" r:id="rId36" xr:uid="{00DC0804-6858-45B8-8BD1-022941C43EAA}"/>
-    <hyperlink ref="E26" r:id="rId37" xr:uid="{6BBA54BF-EC3C-48F0-B95F-DE06F6377104}"/>
-    <hyperlink ref="D26" r:id="rId38" xr:uid="{23BBD2FF-4E49-4E26-BED8-75D6D49D6638}"/>
-    <hyperlink ref="F26" r:id="rId39" xr:uid="{E27B6780-5F75-48CD-B547-7BA3FDA4991E}"/>
-    <hyperlink ref="E28" r:id="rId40" xr:uid="{F3604C68-A129-4E00-8F7F-940340DBF6B9}"/>
-    <hyperlink ref="D28" r:id="rId41" xr:uid="{C1B4D621-AE85-44C9-B0CD-8A6B990282EB}"/>
-    <hyperlink ref="F28" r:id="rId42" xr:uid="{3F612C09-7592-45D0-B2F1-394A3709B286}"/>
-    <hyperlink ref="E31" r:id="rId43" xr:uid="{AE58F565-8771-4E68-A48B-03B303FE7E4A}"/>
-    <hyperlink ref="D31" r:id="rId44" xr:uid="{86C575C4-B2D6-42D6-B237-BE6EBECFF5C1}"/>
-    <hyperlink ref="F31" r:id="rId45" xr:uid="{E92C21A9-6126-492B-83FE-853CBA06E225}"/>
-    <hyperlink ref="D30" r:id="rId46" xr:uid="{7656DEB0-29DF-47CF-B3F2-B11E0BDCD11B}"/>
-    <hyperlink ref="E30" r:id="rId47" xr:uid="{50F402B7-A12D-4535-9C63-4479B10ED9AF}"/>
-    <hyperlink ref="F30" r:id="rId48" xr:uid="{E4115000-88AB-4B63-8360-1D902D24950B}"/>
-    <hyperlink ref="E29" r:id="rId49" xr:uid="{737CA4AD-2345-4B7D-BDFE-F9D8FD43D744}"/>
-    <hyperlink ref="D29" r:id="rId50" xr:uid="{34EFE560-8C3C-41A9-A328-EB7FC69C6FE0}"/>
-    <hyperlink ref="F29" r:id="rId51" xr:uid="{5778BFF0-EA7C-43FE-BF2D-7656F3AE166C}"/>
+    <hyperlink ref="D37" r:id="rId1" xr:uid="{AB31DAB3-9BD1-4F3A-9C67-266253A7FBC9}"/>
+    <hyperlink ref="F37" r:id="rId2" xr:uid="{FA265D1A-7467-4D20-B06B-A57A3A3B9EC0}"/>
+    <hyperlink ref="E37" r:id="rId3" xr:uid="{8D565E7A-162F-4936-A87E-9067AF1B32C5}"/>
+    <hyperlink ref="D13" r:id="rId4" xr:uid="{14A7163B-E0A4-4CF0-8580-81B5F9151720}"/>
+    <hyperlink ref="E13" r:id="rId5" xr:uid="{F387424D-DD4F-4D43-A515-31E7B2F7E60D}"/>
+    <hyperlink ref="F13" r:id="rId6" xr:uid="{3FCC6F7F-7E77-45C4-80F3-37006936007B}"/>
+    <hyperlink ref="F26" r:id="rId7" xr:uid="{961C82C8-9EE0-4CC7-969E-429E97604A44}"/>
+    <hyperlink ref="D26" r:id="rId8" xr:uid="{29E5C07C-485E-4705-86A5-0805773A71FA}"/>
+    <hyperlink ref="E26" r:id="rId9" xr:uid="{845774F5-18E8-48D6-B185-5EADFEDD176A}"/>
+    <hyperlink ref="E42" r:id="rId10" xr:uid="{86FF1527-77B3-40A2-AC7A-466808CD627A}"/>
+    <hyperlink ref="F42" r:id="rId11" xr:uid="{97C35A04-8C6F-4B13-94DA-27ABEF4EA1A8}"/>
+    <hyperlink ref="D42" r:id="rId12" xr:uid="{DD99B592-4376-4718-B535-8D363D6F4F91}"/>
+    <hyperlink ref="E29" r:id="rId13" xr:uid="{43A44B70-53DA-45DC-96A6-100EB60E6E25}"/>
+    <hyperlink ref="D29" r:id="rId14" xr:uid="{3D4DEEB4-BBA8-42D4-86DE-41C6ECAE8658}"/>
+    <hyperlink ref="F29" r:id="rId15" xr:uid="{E4A64751-9876-494E-894F-EEBFD4AAA2DC}"/>
+    <hyperlink ref="E28" r:id="rId16" xr:uid="{59F4CE5E-9EDB-422C-9561-4B989B3F1BB9}"/>
+    <hyperlink ref="D28" r:id="rId17" xr:uid="{79BB2680-5EFF-4125-9139-09B0EA7840A3}"/>
+    <hyperlink ref="F28" r:id="rId18" xr:uid="{3999E02F-5F6D-49A0-B5C2-E49C775D9A0F}"/>
+    <hyperlink ref="E35" r:id="rId19" xr:uid="{902A354B-3B37-401E-AC8F-7E8BEF8D1480}"/>
+    <hyperlink ref="D35" r:id="rId20" xr:uid="{59AE041E-9814-4B37-92D2-6FB6B6358F14}"/>
+    <hyperlink ref="F35" r:id="rId21" xr:uid="{E0EFE0A8-5B37-4341-AE96-D9068EDDDD1D}"/>
+    <hyperlink ref="E33" r:id="rId22" xr:uid="{DD490B8D-8DC3-4D71-9E8A-0ECBF447F2C6}"/>
+    <hyperlink ref="D33" r:id="rId23" xr:uid="{5D43292E-C65D-4235-B9FD-0CEFF1E811F7}"/>
+    <hyperlink ref="F33" r:id="rId24" xr:uid="{04D35B6E-9D8A-4916-9692-3C5F3E598C19}"/>
+    <hyperlink ref="E25" r:id="rId25" xr:uid="{9AA0D1C7-90F7-4A2E-AA56-2F5442EC7372}"/>
+    <hyperlink ref="D25" r:id="rId26" xr:uid="{5CA1E2FE-E496-49DE-AA8F-E09FB87CB01B}"/>
+    <hyperlink ref="F25" r:id="rId27" xr:uid="{80AAC719-1D00-4D06-BCE4-7051130B5E4C}"/>
+    <hyperlink ref="F24" r:id="rId28" xr:uid="{96B8B0E9-437A-4600-888F-086253A894AC}"/>
+    <hyperlink ref="D24" r:id="rId29" xr:uid="{C23ACE2A-9613-465E-9C5F-D0DB9CB85A71}"/>
+    <hyperlink ref="E24" r:id="rId30" xr:uid="{8E3C6832-26BE-4E46-BB46-BC801F2F73B4}"/>
+    <hyperlink ref="E34" r:id="rId31" xr:uid="{7F34C4E1-B864-4826-9C06-D9B5AC94F1E8}"/>
+    <hyperlink ref="D34" r:id="rId32" xr:uid="{38FF4FD6-EE0D-4CB9-A9A3-48FF37E7358D}"/>
+    <hyperlink ref="F34" r:id="rId33" xr:uid="{1533D866-2B4B-47F8-8F74-C3C814BBBD09}"/>
+    <hyperlink ref="D5" r:id="rId34" xr:uid="{AC2B16DC-1EC4-4B44-A10B-3930A7203AAD}"/>
+    <hyperlink ref="E5" r:id="rId35" xr:uid="{AB5148A2-9F1E-4BDC-8A6B-8FAE98A5E4B5}"/>
+    <hyperlink ref="F5" r:id="rId36" xr:uid="{00DC0804-6858-45B8-8BD1-022941C43EAA}"/>
+    <hyperlink ref="E4" r:id="rId37" xr:uid="{6BBA54BF-EC3C-48F0-B95F-DE06F6377104}"/>
+    <hyperlink ref="D4" r:id="rId38" xr:uid="{23BBD2FF-4E49-4E26-BED8-75D6D49D6638}"/>
+    <hyperlink ref="F4" r:id="rId39" xr:uid="{E27B6780-5F75-48CD-B547-7BA3FDA4991E}"/>
+    <hyperlink ref="E6" r:id="rId40" xr:uid="{F3604C68-A129-4E00-8F7F-940340DBF6B9}"/>
+    <hyperlink ref="D6" r:id="rId41" xr:uid="{C1B4D621-AE85-44C9-B0CD-8A6B990282EB}"/>
+    <hyperlink ref="F6" r:id="rId42" xr:uid="{3F612C09-7592-45D0-B2F1-394A3709B286}"/>
+    <hyperlink ref="E9" r:id="rId43" xr:uid="{AE58F565-8771-4E68-A48B-03B303FE7E4A}"/>
+    <hyperlink ref="D9" r:id="rId44" xr:uid="{86C575C4-B2D6-42D6-B237-BE6EBECFF5C1}"/>
+    <hyperlink ref="F9" r:id="rId45" xr:uid="{E92C21A9-6126-492B-83FE-853CBA06E225}"/>
+    <hyperlink ref="D8" r:id="rId46" xr:uid="{7656DEB0-29DF-47CF-B3F2-B11E0BDCD11B}"/>
+    <hyperlink ref="E8" r:id="rId47" xr:uid="{50F402B7-A12D-4535-9C63-4479B10ED9AF}"/>
+    <hyperlink ref="F8" r:id="rId48" xr:uid="{E4115000-88AB-4B63-8360-1D902D24950B}"/>
+    <hyperlink ref="E7" r:id="rId49" xr:uid="{737CA4AD-2345-4B7D-BDFE-F9D8FD43D744}"/>
+    <hyperlink ref="D7" r:id="rId50" xr:uid="{34EFE560-8C3C-41A9-A328-EB7FC69C6FE0}"/>
+    <hyperlink ref="F7" r:id="rId51" xr:uid="{5778BFF0-EA7C-43FE-BF2D-7656F3AE166C}"/>
     <hyperlink ref="E3" r:id="rId52" xr:uid="{182FE997-E7B0-4264-B7FA-91488AD1E0E9}"/>
     <hyperlink ref="D3" r:id="rId53" xr:uid="{1797FA80-8971-4E2C-8862-966D75D20048}"/>
     <hyperlink ref="F3" r:id="rId54" xr:uid="{7D641387-B8BD-48B1-9054-37FA80DE2029}"/>
-    <hyperlink ref="E33" r:id="rId55" xr:uid="{57666301-DAFC-4D67-BC2B-9A6DE0A2BE0D}"/>
-    <hyperlink ref="D33" r:id="rId56" xr:uid="{A0709C3B-BC30-461E-B72E-031657C5A3E7}"/>
-    <hyperlink ref="F33" r:id="rId57" xr:uid="{D44FED01-47D7-4BB2-BC25-E0BFC39F8F73}"/>
-    <hyperlink ref="D34" r:id="rId58" xr:uid="{1A85AE11-5156-45A9-A622-085497CFE9B8}"/>
-    <hyperlink ref="D35" r:id="rId59" xr:uid="{9E1E8C2E-AD42-47CD-9087-1D092998ADDE}"/>
-    <hyperlink ref="F34" r:id="rId60" xr:uid="{479D741D-9921-4140-8648-688C5C791B90}"/>
-    <hyperlink ref="E34" r:id="rId61" xr:uid="{E287107A-CE53-4339-9601-2AEE217A283F}"/>
-    <hyperlink ref="E35" r:id="rId62" xr:uid="{6436DFBC-2293-47B5-86F7-D1B619E0CE12}"/>
-    <hyperlink ref="F35" r:id="rId63" xr:uid="{DC84A2A0-7EC4-42A9-A3B1-C7042BEF8C9A}"/>
-    <hyperlink ref="D16" r:id="rId64" xr:uid="{C94488F7-07DB-4916-BEA9-B6DB6FDE36DD}"/>
-    <hyperlink ref="E16" r:id="rId65" xr:uid="{F37EFDC9-1DF2-4000-B650-A3B9AE118769}"/>
-    <hyperlink ref="F16" r:id="rId66" xr:uid="{C74C3ECF-0C0C-4068-910C-EAE8554C8620}"/>
-    <hyperlink ref="E10" r:id="rId67" xr:uid="{8765E8E6-EDA0-4C2E-A1E8-0E07CD9C7935}"/>
-    <hyperlink ref="D10" r:id="rId68" xr:uid="{81BE556D-B914-4C78-AA20-3FFDFD97BD4E}"/>
-    <hyperlink ref="F10" r:id="rId69" xr:uid="{C9D91D1F-16B7-41A4-80B1-EA1E649AC4C9}"/>
-    <hyperlink ref="E9" r:id="rId70" xr:uid="{ECEB1367-E0E4-412B-9D28-32EFB1B09DD0}"/>
-    <hyperlink ref="D9" r:id="rId71" xr:uid="{B3857C5C-9B2D-4D2F-AEE8-04DC05D251F2}"/>
-    <hyperlink ref="F9" r:id="rId72" xr:uid="{951EDC12-6E0E-4433-B991-F0DF07B38B57}"/>
-    <hyperlink ref="E14" r:id="rId73" xr:uid="{8910E949-ED00-441E-BC59-9CD6D10BF07F}"/>
-    <hyperlink ref="F14" r:id="rId74" xr:uid="{F11EC8A9-F1E4-4D94-9EDF-61966CD73F82}"/>
-    <hyperlink ref="D14" r:id="rId75" xr:uid="{3C2A37B6-2C5B-4B7A-BFA7-C1710C2F8103}"/>
-    <hyperlink ref="E11" r:id="rId76" xr:uid="{018328DA-78D8-43DF-A106-0A8D93E9D48F}"/>
-    <hyperlink ref="D11" r:id="rId77" xr:uid="{3AFC31C7-F940-4DD2-BC94-06DF9CB93B56}"/>
-    <hyperlink ref="F11" r:id="rId78" xr:uid="{EBB781CA-B554-43B2-8815-1253BDA6EA85}"/>
-    <hyperlink ref="E38" r:id="rId79" xr:uid="{19E794AE-569C-4152-92EF-525B510EA0A2}"/>
-    <hyperlink ref="D38" r:id="rId80" xr:uid="{31651AB9-7ACB-49DC-9A2E-E46BAFC49A19}"/>
-    <hyperlink ref="F38" r:id="rId81" xr:uid="{5EB1ACCD-F9CE-495A-84D1-7A96020AA929}"/>
-    <hyperlink ref="E13" r:id="rId82" xr:uid="{DE4A266B-EA65-4441-BC67-90301F73FE0A}"/>
-    <hyperlink ref="D13" r:id="rId83" xr:uid="{097F42E2-DB56-421C-BF2B-64676D013847}"/>
-    <hyperlink ref="F13" r:id="rId84" xr:uid="{899F4FA9-0E0C-446C-A5A4-6E0FF5E7AF87}"/>
-    <hyperlink ref="E4" r:id="rId85" xr:uid="{7E33C556-C47B-4EAB-A88A-7DD3F1326A84}"/>
-    <hyperlink ref="D4" r:id="rId86" xr:uid="{3AAB6DD8-B4EA-400A-AE72-603B7FE17A97}"/>
-    <hyperlink ref="D23" r:id="rId87" xr:uid="{D9D90F66-21BE-4C05-BF81-8769D91956FC}"/>
-    <hyperlink ref="E23" r:id="rId88" xr:uid="{DBDC2A88-3B09-453B-96C8-F90F11547517}"/>
-    <hyperlink ref="F23" r:id="rId89" xr:uid="{0ED2AC43-4B61-4F30-A4C2-D557CD2C2FB2}"/>
-    <hyperlink ref="F4" r:id="rId90" xr:uid="{D008DE06-1825-44B9-B279-ED6DEBFC2302}"/>
-    <hyperlink ref="E32" r:id="rId91" xr:uid="{159D8439-754A-4083-8163-2B0BB64FC61E}"/>
-    <hyperlink ref="D32" r:id="rId92" xr:uid="{40F6B21B-C883-4DC0-90BC-903719FF73D5}"/>
-    <hyperlink ref="F32" r:id="rId93" xr:uid="{89882F9C-A31C-4792-B8CD-57E27E2DA9C5}"/>
-    <hyperlink ref="E25" r:id="rId94" xr:uid="{DE947725-211C-4E57-B345-AEEF9E842913}"/>
-    <hyperlink ref="D25" r:id="rId95" xr:uid="{1DA375B6-2C1B-4B5B-80C3-B72F54168AB4}"/>
-    <hyperlink ref="E24" r:id="rId96" xr:uid="{968FA50A-AD92-459F-A14E-FA090F288EA1}"/>
-    <hyperlink ref="F25" r:id="rId97" xr:uid="{7ADDC187-F89E-4FE0-9AE8-3DAC280959E6}"/>
-    <hyperlink ref="F24" r:id="rId98" xr:uid="{3564A8FE-606D-4A57-AAC6-1CA45B3FA4EE}"/>
-    <hyperlink ref="D24" r:id="rId99" xr:uid="{0034CD97-470B-4F26-9BFB-B3A24354C52D}"/>
-    <hyperlink ref="E20" r:id="rId100" xr:uid="{9FAAEB72-BF70-415E-9B0F-A5FEAAFA3A7F}"/>
-    <hyperlink ref="D20" r:id="rId101" xr:uid="{A2B16E68-8A46-4635-B8A8-774A5B9BDEFE}"/>
-    <hyperlink ref="F20" r:id="rId102" xr:uid="{E51810B6-7751-441D-A1A4-D96E61532AB3}"/>
-    <hyperlink ref="E2" r:id="rId103" xr:uid="{F4AAE2ED-602C-491B-A957-0B791195FF18}"/>
-    <hyperlink ref="D2" r:id="rId104" xr:uid="{3464D772-267A-451A-9D29-69C94ED1FDF6}"/>
-    <hyperlink ref="F2" r:id="rId105" xr:uid="{C788A329-90C5-4E47-BD7B-A0BB54E52A6F}"/>
-    <hyperlink ref="E5" r:id="rId106" xr:uid="{D167231C-58DE-4853-B259-5CBD05DC2863}"/>
-    <hyperlink ref="D5" r:id="rId107" xr:uid="{4D4349AB-1A12-4FF9-BF7D-A2CE914A74E7}"/>
-    <hyperlink ref="F5" r:id="rId108" xr:uid="{64D1B2F1-9396-443B-987F-A4539E782C4C}"/>
-    <hyperlink ref="E21" r:id="rId109" xr:uid="{2C47B39F-CC7C-44B7-B071-9DE285CE8D4B}"/>
-    <hyperlink ref="D21" r:id="rId110" xr:uid="{6B6D8024-B88D-47D9-89BB-B5E601BF520D}"/>
-    <hyperlink ref="F21" r:id="rId111" xr:uid="{33750801-8F5B-49F0-B6F8-27DB77AF6505}"/>
-    <hyperlink ref="E15" r:id="rId112" xr:uid="{3D588524-D705-4C34-8057-58E931E0DFF7}"/>
-    <hyperlink ref="D15" r:id="rId113" xr:uid="{28C4E742-D754-42AA-8434-496C36B921FC}"/>
-    <hyperlink ref="F15" r:id="rId114" xr:uid="{11FEECD5-1D5D-40E7-9342-FB566C8FAD83}"/>
-    <hyperlink ref="E39" r:id="rId115" xr:uid="{643CF298-FAB8-4D7B-A868-480DE588628B}"/>
-    <hyperlink ref="D39" r:id="rId116" xr:uid="{2400831D-3FEB-4299-AC86-B1F79044C0F2}"/>
-    <hyperlink ref="F39" r:id="rId117" xr:uid="{1780D338-C96B-42CB-A7C2-E33C200AB344}"/>
-    <hyperlink ref="D6" r:id="rId118" xr:uid="{0AD478D4-457D-43C6-8C86-6CD72283A3E0}"/>
-    <hyperlink ref="F6" r:id="rId119" xr:uid="{54DBC843-9C87-404B-A9E8-77C4337A1522}"/>
-    <hyperlink ref="E6" r:id="rId120" xr:uid="{43D41189-14E5-45F8-9FDE-B09D5240C6D4}"/>
-    <hyperlink ref="D8" r:id="rId121" xr:uid="{579319CA-001E-47B8-A2A2-5F2E264DE279}"/>
-    <hyperlink ref="E8" r:id="rId122" xr:uid="{4755B706-AFD2-4397-9FA9-A84859413B61}"/>
-    <hyperlink ref="F8" r:id="rId123" xr:uid="{754234A8-FC70-4A6D-AFC2-BC5CB3428305}"/>
+    <hyperlink ref="E10" r:id="rId55" xr:uid="{57666301-DAFC-4D67-BC2B-9A6DE0A2BE0D}"/>
+    <hyperlink ref="D10" r:id="rId56" xr:uid="{A0709C3B-BC30-461E-B72E-031657C5A3E7}"/>
+    <hyperlink ref="F10" r:id="rId57" xr:uid="{D44FED01-47D7-4BB2-BC25-E0BFC39F8F73}"/>
+    <hyperlink ref="D11" r:id="rId58" xr:uid="{1A85AE11-5156-45A9-A622-085497CFE9B8}"/>
+    <hyperlink ref="D12" r:id="rId59" xr:uid="{9E1E8C2E-AD42-47CD-9087-1D092998ADDE}"/>
+    <hyperlink ref="F11" r:id="rId60" xr:uid="{479D741D-9921-4140-8648-688C5C791B90}"/>
+    <hyperlink ref="E11" r:id="rId61" xr:uid="{E287107A-CE53-4339-9601-2AEE217A283F}"/>
+    <hyperlink ref="E12" r:id="rId62" xr:uid="{6436DFBC-2293-47B5-86F7-D1B619E0CE12}"/>
+    <hyperlink ref="F12" r:id="rId63" xr:uid="{DC84A2A0-7EC4-42A9-A3B1-C7042BEF8C9A}"/>
+    <hyperlink ref="D27" r:id="rId64" xr:uid="{C94488F7-07DB-4916-BEA9-B6DB6FDE36DD}"/>
+    <hyperlink ref="E27" r:id="rId65" xr:uid="{F37EFDC9-1DF2-4000-B650-A3B9AE118769}"/>
+    <hyperlink ref="F27" r:id="rId66" xr:uid="{C74C3ECF-0C0C-4068-910C-EAE8554C8620}"/>
+    <hyperlink ref="E23" r:id="rId67" xr:uid="{8765E8E6-EDA0-4C2E-A1E8-0E07CD9C7935}"/>
+    <hyperlink ref="D23" r:id="rId68" xr:uid="{81BE556D-B914-4C78-AA20-3FFDFD97BD4E}"/>
+    <hyperlink ref="F23" r:id="rId69" xr:uid="{C9D91D1F-16B7-41A4-80B1-EA1E649AC4C9}"/>
+    <hyperlink ref="E22" r:id="rId70" xr:uid="{ECEB1367-E0E4-412B-9D28-32EFB1B09DD0}"/>
+    <hyperlink ref="D22" r:id="rId71" xr:uid="{B3857C5C-9B2D-4D2F-AEE8-04DC05D251F2}"/>
+    <hyperlink ref="F22" r:id="rId72" xr:uid="{951EDC12-6E0E-4433-B991-F0DF07B38B57}"/>
+    <hyperlink ref="E20" r:id="rId73" xr:uid="{8910E949-ED00-441E-BC59-9CD6D10BF07F}"/>
+    <hyperlink ref="F20" r:id="rId74" xr:uid="{F11EC8A9-F1E4-4D94-9EDF-61966CD73F82}"/>
+    <hyperlink ref="D20" r:id="rId75" xr:uid="{3C2A37B6-2C5B-4B7A-BFA7-C1710C2F8103}"/>
+    <hyperlink ref="E19" r:id="rId76" xr:uid="{018328DA-78D8-43DF-A106-0A8D93E9D48F}"/>
+    <hyperlink ref="D19" r:id="rId77" xr:uid="{3AFC31C7-F940-4DD2-BC94-06DF9CB93B56}"/>
+    <hyperlink ref="F19" r:id="rId78" xr:uid="{EBB781CA-B554-43B2-8815-1253BDA6EA85}"/>
+    <hyperlink ref="E21" r:id="rId79" xr:uid="{19E794AE-569C-4152-92EF-525B510EA0A2}"/>
+    <hyperlink ref="D21" r:id="rId80" xr:uid="{31651AB9-7ACB-49DC-9A2E-E46BAFC49A19}"/>
+    <hyperlink ref="F21" r:id="rId81" xr:uid="{5EB1ACCD-F9CE-495A-84D1-7A96020AA929}"/>
+    <hyperlink ref="E30" r:id="rId82" xr:uid="{DE4A266B-EA65-4441-BC67-90301F73FE0A}"/>
+    <hyperlink ref="D30" r:id="rId83" xr:uid="{097F42E2-DB56-421C-BF2B-64676D013847}"/>
+    <hyperlink ref="F30" r:id="rId84" xr:uid="{899F4FA9-0E0C-446C-A5A4-6E0FF5E7AF87}"/>
+    <hyperlink ref="E14" r:id="rId85" xr:uid="{7E33C556-C47B-4EAB-A88A-7DD3F1326A84}"/>
+    <hyperlink ref="D14" r:id="rId86" xr:uid="{3AAB6DD8-B4EA-400A-AE72-603B7FE17A97}"/>
+    <hyperlink ref="D15" r:id="rId87" xr:uid="{D9D90F66-21BE-4C05-BF81-8769D91956FC}"/>
+    <hyperlink ref="E15" r:id="rId88" xr:uid="{DBDC2A88-3B09-453B-96C8-F90F11547517}"/>
+    <hyperlink ref="F15" r:id="rId89" xr:uid="{0ED2AC43-4B61-4F30-A4C2-D557CD2C2FB2}"/>
+    <hyperlink ref="F14" r:id="rId90" xr:uid="{D008DE06-1825-44B9-B279-ED6DEBFC2302}"/>
+    <hyperlink ref="E18" r:id="rId91" xr:uid="{159D8439-754A-4083-8163-2B0BB64FC61E}"/>
+    <hyperlink ref="D18" r:id="rId92" xr:uid="{40F6B21B-C883-4DC0-90BC-903719FF73D5}"/>
+    <hyperlink ref="F18" r:id="rId93" xr:uid="{89882F9C-A31C-4792-B8CD-57E27E2DA9C5}"/>
+    <hyperlink ref="E17" r:id="rId94" xr:uid="{DE947725-211C-4E57-B345-AEEF9E842913}"/>
+    <hyperlink ref="D17" r:id="rId95" xr:uid="{1DA375B6-2C1B-4B5B-80C3-B72F54168AB4}"/>
+    <hyperlink ref="E16" r:id="rId96" xr:uid="{968FA50A-AD92-459F-A14E-FA090F288EA1}"/>
+    <hyperlink ref="F17" r:id="rId97" xr:uid="{7ADDC187-F89E-4FE0-9AE8-3DAC280959E6}"/>
+    <hyperlink ref="F16" r:id="rId98" xr:uid="{3564A8FE-606D-4A57-AAC6-1CA45B3FA4EE}"/>
+    <hyperlink ref="D16" r:id="rId99" xr:uid="{0034CD97-470B-4F26-9BFB-B3A24354C52D}"/>
+    <hyperlink ref="E40" r:id="rId100" xr:uid="{9FAAEB72-BF70-415E-9B0F-A5FEAAFA3A7F}"/>
+    <hyperlink ref="D40" r:id="rId101" xr:uid="{A2B16E68-8A46-4635-B8A8-774A5B9BDEFE}"/>
+    <hyperlink ref="F40" r:id="rId102" xr:uid="{E51810B6-7751-441D-A1A4-D96E61532AB3}"/>
+    <hyperlink ref="E38" r:id="rId103" xr:uid="{F4AAE2ED-602C-491B-A957-0B791195FF18}"/>
+    <hyperlink ref="D38" r:id="rId104" xr:uid="{3464D772-267A-451A-9D29-69C94ED1FDF6}"/>
+    <hyperlink ref="F38" r:id="rId105" xr:uid="{C788A329-90C5-4E47-BD7B-A0BB54E52A6F}"/>
+    <hyperlink ref="E39" r:id="rId106" xr:uid="{D167231C-58DE-4853-B259-5CBD05DC2863}"/>
+    <hyperlink ref="D39" r:id="rId107" xr:uid="{4D4349AB-1A12-4FF9-BF7D-A2CE914A74E7}"/>
+    <hyperlink ref="F39" r:id="rId108" xr:uid="{64D1B2F1-9396-443B-987F-A4539E782C4C}"/>
+    <hyperlink ref="E41" r:id="rId109" xr:uid="{2C47B39F-CC7C-44B7-B071-9DE285CE8D4B}"/>
+    <hyperlink ref="D41" r:id="rId110" xr:uid="{6B6D8024-B88D-47D9-89BB-B5E601BF520D}"/>
+    <hyperlink ref="F41" r:id="rId111" xr:uid="{33750801-8F5B-49F0-B6F8-27DB77AF6505}"/>
+    <hyperlink ref="E32" r:id="rId112" xr:uid="{3D588524-D705-4C34-8057-58E931E0DFF7}"/>
+    <hyperlink ref="D32" r:id="rId113" xr:uid="{28C4E742-D754-42AA-8434-496C36B921FC}"/>
+    <hyperlink ref="F32" r:id="rId114" xr:uid="{11FEECD5-1D5D-40E7-9342-FB566C8FAD83}"/>
+    <hyperlink ref="E2" r:id="rId115" xr:uid="{643CF298-FAB8-4D7B-A868-480DE588628B}"/>
+    <hyperlink ref="D2" r:id="rId116" xr:uid="{2400831D-3FEB-4299-AC86-B1F79044C0F2}"/>
+    <hyperlink ref="F2" r:id="rId117" xr:uid="{1780D338-C96B-42CB-A7C2-E33C200AB344}"/>
+    <hyperlink ref="D31" r:id="rId118" xr:uid="{0AD478D4-457D-43C6-8C86-6CD72283A3E0}"/>
+    <hyperlink ref="F31" r:id="rId119" xr:uid="{54DBC843-9C87-404B-A9E8-77C4337A1522}"/>
+    <hyperlink ref="E31" r:id="rId120" xr:uid="{43D41189-14E5-45F8-9FDE-B09D5240C6D4}"/>
+    <hyperlink ref="D36" r:id="rId121" xr:uid="{579319CA-001E-47B8-A2A2-5F2E264DE279}"/>
+    <hyperlink ref="E36" r:id="rId122" xr:uid="{4755B706-AFD2-4397-9FA9-A84859413B61}"/>
+    <hyperlink ref="F36" r:id="rId123" xr:uid="{754234A8-FC70-4A6D-AFC2-BC5CB3428305}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId124"/>

</xml_diff>